<commit_message>
update result about impact of static feautres
</commit_message>
<xml_diff>
--- a/Experimental results/Intrinsic analysis.xlsx
+++ b/Experimental results/Intrinsic analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thu-trangnguyen/Documents/Projects/PEARL/Experimental results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74219B5E-50FD-1048-8D09-C0000637E0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0342FEC2-AE8C-9C4C-8B9C-83E412CBCEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intrinsic analysis" sheetId="3" r:id="rId1"/>
@@ -375,24 +375,6 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -449,12 +431,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -470,10 +446,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -697,7 +697,7 @@
   <dimension ref="A3:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -707,22 +707,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="78"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
@@ -737,8 +737,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="80" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -755,8 +755,8 @@
         <v>0.4444841011364386</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="26"/>
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="75"/>
       <c r="B7" s="13" t="s">
         <v>6</v>
       </c>
@@ -772,22 +772,22 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C11" s="78"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>2</v>
       </c>
@@ -802,8 +802,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="80" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="13" t="s">
@@ -822,8 +822,8 @@
       <c r="F13" s="9"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="26"/>
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="75"/>
       <c r="B14" s="13" t="s">
         <v>6</v>
       </c>
@@ -838,39 +838,39 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="24"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="43">
+      <c r="B19" s="35">
         <v>5</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19" s="35">
         <v>10</v>
       </c>
-      <c r="D19" s="43">
+      <c r="D19" s="35">
         <v>20</v>
       </c>
-      <c r="E19" s="43">
+      <c r="E19" s="35">
         <v>30</v>
       </c>
-      <c r="F19" s="43">
+      <c r="F19" s="35">
         <v>40</v>
       </c>
-      <c r="G19" s="43">
+      <c r="G19" s="35">
         <v>50</v>
       </c>
     </row>
@@ -898,7 +898,7 @@
         <f>(0.6582694982+0.6484626903)/2</f>
         <v>0.65336609425000003</v>
       </c>
-      <c r="G20" s="59">
+      <c r="G20" s="51">
         <f>(0.6595980984+0.6501529501)/2</f>
         <v>0.65487552424999995</v>
       </c>
@@ -927,7 +927,7 @@
         <f>(0.7903510411+0.7704737321)/2</f>
         <v>0.78041238660000001</v>
       </c>
-      <c r="G21" s="59">
+      <c r="G21" s="51">
         <f>(0.7922712836+0.7725957431)/2</f>
         <v>0.78243351335</v>
       </c>
@@ -956,7 +956,7 @@
         <f>(0.8196321438+0.7991989638)/2</f>
         <v>0.80941555380000008</v>
       </c>
-      <c r="G22" s="59">
+      <c r="G22" s="51">
         <f>(0.8216146644+0.8014403954)/2</f>
         <v>0.81152752989999999</v>
       </c>
@@ -964,131 +964,131 @@
       <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="51">
+      <c r="B23" s="43">
         <f>(0.8280293122+0.8115543961)/2</f>
         <v>0.81979185415</v>
       </c>
-      <c r="C23" s="51">
+      <c r="C23" s="43">
         <f>(0.8297627203+0.8124913879)/2</f>
         <v>0.82112705409999998</v>
       </c>
-      <c r="D23" s="51">
+      <c r="D23" s="43">
         <f>(0.8352535758+0.8164598242)/2</f>
         <v>0.8258567</v>
       </c>
-      <c r="E23" s="51">
+      <c r="E23" s="43">
         <f>(0.8390836811+0.8193075446)/2</f>
         <v>0.82919561284999999</v>
       </c>
-      <c r="F23" s="52">
+      <c r="F23" s="44">
         <f>(0.8417097424+0.8216132796)/2</f>
         <v>0.83166151099999996</v>
       </c>
-      <c r="G23" s="60">
+      <c r="G23" s="52">
         <f>(0.8433704926+0.8233954014)/2</f>
         <v>0.83338294700000004</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="A24" s="53" t="s">
+      <c r="A24" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="55">
+      <c r="C24" s="47">
         <f>(0.295870244195522+0.259468318982455)/2+0.0239210891623016+0.04</f>
         <v>0.34159037075129012</v>
       </c>
-      <c r="D24" s="56">
+      <c r="D24" s="48">
         <f>(0.351753974045934+0.333310216409888)/2+0.0239210891623016+0.04</f>
         <v>0.40645318439021261</v>
       </c>
-      <c r="E24" s="56">
+      <c r="E24" s="48">
         <f>(0.370334290897527+0.337867129229664)/2+0.0239210891623016+0.04</f>
         <v>0.41802179922589711</v>
       </c>
-      <c r="F24" s="57">
+      <c r="F24" s="49">
         <f>(0.414963749591282+0.3849658073126)/2+0.0239210891623016+0.04</f>
         <v>0.46388586761424261</v>
       </c>
-      <c r="G24" s="58">
+      <c r="G24" s="50">
         <f>(0.461205554246172+0.426161937390751)/2+0.0239210891623016+0.04</f>
         <v>0.50760483498076314</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="A25" s="48"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="46"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="38"/>
     </row>
     <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="A26" s="48"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="46"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="38"/>
     </row>
     <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="71" t="s">
+      <c r="A27" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="70"/>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="46"/>
+      <c r="B27" s="77"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="38"/>
     </row>
     <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="F28" s="45"/>
-      <c r="G28" s="46"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="38"/>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="67"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="68" t="s">
+      <c r="A29" s="59"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="68" t="s">
+      <c r="D29" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="68" t="s">
+      <c r="E29" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="45"/>
-      <c r="G29" s="46"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="38"/>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="63" t="s">
+      <c r="B30" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="64">
+      <c r="C30" s="56">
         <v>0.70709999999999995</v>
       </c>
-      <c r="D30" s="65">
+      <c r="D30" s="57">
         <v>0.76</v>
       </c>
-      <c r="E30" s="66">
+      <c r="E30" s="58">
         <v>0.73199999999999998</v>
       </c>
-      <c r="F30" s="45"/>
-      <c r="G30" s="46"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="38"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="28"/>
+      <c r="A31" s="74"/>
       <c r="B31" s="19" t="s">
         <v>6</v>
       </c>
@@ -1103,7 +1103,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="28"/>
+      <c r="A32" s="74"/>
       <c r="B32" s="19" t="s">
         <v>19</v>
       </c>
@@ -1118,7 +1118,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="26"/>
+      <c r="A33" s="75"/>
       <c r="B33" s="19" t="s">
         <v>7</v>
       </c>
@@ -1133,35 +1133,35 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="A34" s="48"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
     </row>
     <row r="35" spans="1:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="A35" s="48"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="82" t="s">
+      <c r="A36" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="81"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="44"/>
-    </row>
-    <row r="37" spans="1:7" s="78" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="61"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="79"/>
-      <c r="D37" s="80"/>
-    </row>
-    <row r="38" spans="1:7" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="82"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="36"/>
+    </row>
+    <row r="37" spans="1:7" s="68" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="53"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="70"/>
+    </row>
+    <row r="38" spans="1:7" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
         <v>23</v>
       </c>
@@ -1178,8 +1178,8 @@
       <c r="F38"/>
       <c r="G38"/>
     </row>
-    <row r="39" spans="1:7" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="29" t="s">
+    <row r="39" spans="1:7" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="80" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="13" t="s">
@@ -1195,8 +1195,8 @@
       <c r="F39"/>
       <c r="G39"/>
     </row>
-    <row r="40" spans="1:7" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="26"/>
+    <row r="40" spans="1:7" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="75"/>
       <c r="B40" s="13" t="s">
         <v>6</v>
       </c>
@@ -1210,210 +1210,230 @@
       <c r="F40"/>
       <c r="G40"/>
     </row>
-    <row r="41" spans="1:7" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="29" t="s">
+    <row r="41" spans="1:7" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="80" t="s">
         <v>19</v>
       </c>
       <c r="B41" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="15"/>
+      <c r="C41" s="14">
+        <v>0.3664</v>
+      </c>
+      <c r="D41" s="15">
+        <v>0.51400000000000001</v>
+      </c>
       <c r="E41"/>
       <c r="F41"/>
       <c r="G41"/>
     </row>
-    <row r="42" spans="1:7" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="26"/>
+    <row r="42" spans="1:7" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="75"/>
       <c r="B42" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="15"/>
+      <c r="C42" s="14">
+        <v>0.25190000000000001</v>
+      </c>
+      <c r="D42" s="15">
+        <v>0.442</v>
+      </c>
       <c r="E42"/>
       <c r="F42"/>
       <c r="G42"/>
     </row>
-    <row r="43" spans="1:7" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="29" t="s">
+    <row r="43" spans="1:7" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="80" t="s">
         <v>7</v>
       </c>
       <c r="B43" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="15"/>
+      <c r="C43" s="14">
+        <v>0.3584</v>
+      </c>
+      <c r="D43" s="15">
+        <v>0.46700000000000003</v>
+      </c>
       <c r="E43"/>
       <c r="F43"/>
       <c r="G43"/>
     </row>
-    <row r="44" spans="1:7" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="26"/>
+    <row r="44" spans="1:7" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="75"/>
       <c r="B44" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="69"/>
+      <c r="C44" s="14">
+        <v>0.29909999999999998</v>
+      </c>
+      <c r="D44" s="15">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="E44" s="61"/>
       <c r="F44"/>
       <c r="G44"/>
     </row>
-    <row r="45" spans="1:7" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="72"/>
-      <c r="B45" s="72"/>
-      <c r="C45" s="73"/>
-      <c r="D45" s="73"/>
-      <c r="E45" s="73"/>
+    <row r="45" spans="1:7" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="62"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="63"/>
       <c r="F45"/>
       <c r="G45"/>
     </row>
-    <row r="46" spans="1:7" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="77"/>
-      <c r="B46" s="72"/>
-      <c r="C46" s="74"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="75"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
+    <row r="46" spans="1:7" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="67"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="64"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="69"/>
-      <c r="B47" s="72"/>
-      <c r="C47" s="74"/>
-      <c r="D47" s="73"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
+      <c r="A47" s="61"/>
+      <c r="B47" s="62"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="65"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="69"/>
-      <c r="B48" s="72"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="76"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
+      <c r="A48" s="61"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="77"/>
-      <c r="B49" s="72"/>
-      <c r="C49" s="74"/>
-      <c r="D49" s="73"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="41"/>
+      <c r="A49" s="67"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="65"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="33"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="69"/>
-      <c r="B50" s="72"/>
-      <c r="C50" s="74"/>
-      <c r="D50" s="73"/>
-      <c r="E50" s="75"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="39"/>
+      <c r="A50" s="61"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="64"/>
+      <c r="D50" s="63"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="69"/>
-      <c r="B51" s="72"/>
-      <c r="C51" s="39"/>
-      <c r="D51" s="76"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="39"/>
+      <c r="A51" s="61"/>
+      <c r="B51" s="62"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="66"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="77"/>
-      <c r="B52" s="72"/>
-      <c r="C52" s="74"/>
-      <c r="D52" s="73"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="39"/>
+      <c r="A52" s="67"/>
+      <c r="B52" s="62"/>
+      <c r="C52" s="64"/>
+      <c r="D52" s="63"/>
+      <c r="E52" s="65"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="69"/>
-      <c r="B53" s="72"/>
-      <c r="C53" s="74"/>
-      <c r="D53" s="73"/>
-      <c r="E53" s="75"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
+      <c r="A53" s="61"/>
+      <c r="B53" s="62"/>
+      <c r="C53" s="64"/>
+      <c r="D53" s="63"/>
+      <c r="E53" s="65"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="30"/>
     </row>
     <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="69"/>
-      <c r="B54" s="72"/>
-      <c r="C54" s="39"/>
-      <c r="D54" s="76"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="36"/>
+      <c r="A54" s="61"/>
+      <c r="B54" s="62"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="66"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
     </row>
     <row r="55" spans="1:7" ht="13" x14ac:dyDescent="0.15"/>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="34"/>
-      <c r="B57" s="35"/>
-      <c r="C57" s="35"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="37"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
+      <c r="A58" s="29"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="37"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="39"/>
-      <c r="E59" s="39"/>
+      <c r="A59" s="29"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="37"/>
-      <c r="B60" s="35"/>
-      <c r="C60" s="40"/>
-      <c r="D60" s="41"/>
-      <c r="E60" s="40"/>
+      <c r="A60" s="29"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="33"/>
+      <c r="E60" s="32"/>
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="35"/>
-      <c r="B61" s="35"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
+      <c r="A61" s="27"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="37"/>
-      <c r="B62" s="35"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="39"/>
+      <c r="A62" s="29"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="31"/>
     </row>
     <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="37"/>
-      <c r="B63" s="35"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="42"/>
-      <c r="E63" s="39"/>
+      <c r="A63" s="29"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="31"/>
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="37"/>
-      <c r="B64" s="35"/>
-      <c r="C64" s="39"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="42"/>
+      <c r="A64" s="29"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="36"/>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
+      <c r="A65" s="28"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A43:A44"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A17:G17"/>
@@ -1423,10 +1443,6 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A43:A44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>